<commit_message>
update report template and query limit
</commit_message>
<xml_diff>
--- a/Report/drycon.xlsx
+++ b/Report/drycon.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24750" windowHeight="10430" activeTab="1"/>
+    <workbookView windowWidth="24750" windowHeight="10430"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="6" r:id="rId1"/>
@@ -1135,12 +1135,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1361,17 +1360,9 @@
         <color theme="0"/>
       </font>
       <fill>
-        <gradientFill>
-          <stop position="0">
-            <color rgb="FFFF0000"/>
-          </stop>
-          <stop position="0.5">
-            <color rgb="FFFB5503"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FFFF0000"/>
-          </stop>
-        </gradientFill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
       </fill>
     </dxf>
   </dxfs>
@@ -1394,40 +1385,33 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>68580</xdr:colOff>
+      <xdr:colOff>121285</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>358775</xdr:colOff>
+      <xdr:colOff>416560</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="3" name="Picture 4" descr="logo"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect t="33684" b="27157"/>
+        <a:blip r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="68580" y="191770"/>
-          <a:ext cx="1097280" cy="344170"/>
+          <a:off x="121285" y="209550"/>
+          <a:ext cx="1102360" cy="339725"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1699,8 +1683,8 @@
   <sheetPr/>
   <dimension ref="A2:K54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20:E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -1718,35 +1702,35 @@
       </c>
     </row>
     <row r="3" spans="3:3">
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" ht="15.5" spans="1:10">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="57"/>
-      <c r="J5" s="58"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="56"/>
+      <c r="J5" s="57"/>
     </row>
     <row r="6" ht="15.5" spans="1:10">
-      <c r="A6" s="9"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="59"/>
-      <c r="J6" s="58"/>
+      <c r="A6" s="8"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="57"/>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
@@ -1769,821 +1753,821 @@
     </row>
     <row r="10" ht="15.25"/>
     <row r="11" ht="28.8" customHeight="1" spans="1:9">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="14" t="s">
+      <c r="C11" s="12"/>
+      <c r="D11" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="16" t="s">
+      <c r="E11" s="14"/>
+      <c r="F11" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="17" t="s">
+      <c r="G11" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="18"/>
-      <c r="I11" s="60"/>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="19"/>
-      <c r="B12" s="20" t="s">
+      <c r="H11" s="17"/>
+      <c r="I11" s="59"/>
+    </row>
+    <row r="12" ht="15.25" spans="1:9">
+      <c r="A12" s="18"/>
+      <c r="B12" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="21"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="61"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="60"/>
     </row>
     <row r="13" ht="15.25" spans="1:9">
-      <c r="A13" s="26" t="str">
+      <c r="A13" s="25" t="str">
         <f>RawData!F3</f>
         <v/>
       </c>
-      <c r="B13" s="27">
+      <c r="B13" s="26">
         <f>_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;A13,RawData!$B$3:$B$6000,"&lt;"&amp;A13+1,RawData!$D$3:$D$6000,"="&amp;B8)</f>
         <v>0</v>
       </c>
-      <c r="C13" s="27">
+      <c r="C13" s="26">
         <f>IF(ISNUMBER(B13),IF(_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;$B13,RawData!$C$3:$C$6000,"&lt;&gt;"&amp;G15,RawData!$B$3:$B$6000,"&lt;"&amp;A$13+1,RawData!$D$3:$D$6000,"="&amp;B$8)&lt;&gt;0,_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;$B13,RawData!$C$3:$C$6000,"&lt;&gt;"&amp;G15,RawData!$B$3:$B$6000,"&lt;"&amp;A$13+1,RawData!$D$3:$D$6000,"="&amp;B$8),MROUND(B$13,1)+1),"")</f>
         <v>1</v>
       </c>
-      <c r="D13" s="28" t="str">
+      <c r="D13" s="27" t="str">
         <f>IF(ISNUMBER(G15),IF(G15=1,"NOT GOOD","GOOD"),"")</f>
         <v/>
       </c>
-      <c r="E13" s="29"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="61"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="60"/>
     </row>
     <row r="14" ht="17" customHeight="1" spans="1:9">
-      <c r="A14" s="30" t="str">
+      <c r="A14" s="29" t="str">
         <f>A13</f>
         <v/>
       </c>
-      <c r="B14" s="31" t="str">
+      <c r="B14" s="30" t="str">
         <f t="shared" ref="B14:B27" si="0">IF(C13&lt;MROUND(B$13,1)+1,C13,"")</f>
         <v/>
       </c>
-      <c r="C14" s="27" t="str">
+      <c r="C14" s="26" t="str">
         <f>IF(ISNUMBER(B14),IF(_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;$B14,RawData!$C$3:$C$6000,"&lt;&gt;"&amp;G16,RawData!$B$3:$B$6000,"&lt;"&amp;A$13+1,RawData!$D$3:$D$6000,"="&amp;B$8)&lt;&gt;0,_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;$B14,RawData!$C$3:$C$6000,"&lt;&gt;"&amp;G16,RawData!$B$3:$B$6000,"&lt;"&amp;A$13+1,RawData!$D$3:$D$6000,"="&amp;B$8),MROUND(B$13,1)+1),"")</f>
         <v/>
       </c>
-      <c r="D14" s="28" t="str">
+      <c r="D14" s="27" t="str">
         <f t="shared" ref="D14:D35" si="1">IF(ISNUMBER(G16),IF(G16=1,"NOT GOOD","GOOD"),"")</f>
         <v/>
       </c>
-      <c r="E14" s="29"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="62"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="61"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="35"/>
-      <c r="B15" s="31" t="str">
+      <c r="A15" s="34"/>
+      <c r="B15" s="30" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C15" s="27" t="str">
+      <c r="C15" s="26" t="str">
         <f>IF(ISNUMBER(B15),IF(_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;$B15,RawData!$C$3:$C$6000,"&lt;&gt;"&amp;G17,RawData!$B$3:$B$6000,"&lt;"&amp;A$13+1,RawData!$D$3:$D$6000,"="&amp;B$8)&lt;&gt;0,_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;$B15,RawData!$C$3:$C$6000,"&lt;&gt;"&amp;G17,RawData!$B$3:$B$6000,"&lt;"&amp;A$13+1,RawData!$D$3:$D$6000,"="&amp;B$8),MROUND(B$13,1)+1),"")</f>
         <v/>
       </c>
-      <c r="D15" s="28" t="str">
+      <c r="D15" s="27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E15" s="29"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="37" t="e">
+      <c r="E15" s="28"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="36" t="e">
         <f>IF(ISNUMBER(B13),VLOOKUP(B13,RawData!$B$3:$D$6000,2,FALSE),"")</f>
         <v>#N/A</v>
       </c>
-      <c r="H15" s="38">
+      <c r="H15" s="37">
         <f t="shared" ref="H15:H37" si="2">IF(ISNUMBER(C13),C13-B13,0)</f>
         <v>1</v>
       </c>
-      <c r="I15" s="63"/>
+      <c r="I15" s="62"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="39"/>
-      <c r="B16" s="31" t="str">
+      <c r="A16" s="38"/>
+      <c r="B16" s="30" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C16" s="27" t="str">
+      <c r="C16" s="26" t="str">
         <f>IF(ISNUMBER(B16),IF(_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;$B16,RawData!$C$3:$C$6000,"&lt;&gt;"&amp;G18,RawData!$B$3:$B$6000,"&lt;"&amp;A$13+1,RawData!$D$3:$D$6000,"="&amp;B$8)&lt;&gt;0,_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;$B16,RawData!$C$3:$C$6000,"&lt;&gt;"&amp;G18,RawData!$B$3:$B$6000,"&lt;"&amp;A$13+1,RawData!$D$3:$D$6000,"="&amp;B$8),MROUND(B$13,1)+1),"")</f>
         <v/>
       </c>
-      <c r="D16" s="28" t="str">
+      <c r="D16" s="27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E16" s="29"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="37" t="str">
+      <c r="E16" s="28"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="36" t="str">
         <f>IF(ISNUMBER(B14),VLOOKUP(B14,RawData!$B$3:$D$6000,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="H16" s="38">
+      <c r="H16" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I16" s="63"/>
+      <c r="I16" s="62"/>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="39"/>
-      <c r="B17" s="31" t="str">
+      <c r="A17" s="38"/>
+      <c r="B17" s="30" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C17" s="27" t="str">
+      <c r="C17" s="26" t="str">
         <f>IF(ISNUMBER(B17),IF(_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;$B17,RawData!$C$3:$C$6000,"&lt;&gt;"&amp;G19,RawData!$B$3:$B$6000,"&lt;"&amp;A$13+1,RawData!$D$3:$D$6000,"="&amp;B$8)&lt;&gt;0,_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;$B17,RawData!$C$3:$C$6000,"&lt;&gt;"&amp;G19,RawData!$B$3:$B$6000,"&lt;"&amp;A$13+1,RawData!$D$3:$D$6000,"="&amp;B$8),MROUND(B$13,1)+1),"")</f>
         <v/>
       </c>
-      <c r="D17" s="28" t="str">
+      <c r="D17" s="27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E17" s="29"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="37" t="str">
+      <c r="E17" s="28"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="36" t="str">
         <f>IF(ISNUMBER(B15),VLOOKUP(B15,RawData!$B$3:$D$6000,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="H17" s="38">
+      <c r="H17" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I17" s="63"/>
+      <c r="I17" s="62"/>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="39"/>
-      <c r="B18" s="31" t="str">
+      <c r="A18" s="38"/>
+      <c r="B18" s="30" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C18" s="27" t="str">
+      <c r="C18" s="26" t="str">
         <f>IF(ISNUMBER(B18),IF(_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;$B18,RawData!$C$3:$C$6000,"&lt;&gt;"&amp;G20,RawData!$B$3:$B$6000,"&lt;"&amp;A$13+1,RawData!$D$3:$D$6000,"="&amp;B$8)&lt;&gt;0,_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;$B18,RawData!$C$3:$C$6000,"&lt;&gt;"&amp;G20,RawData!$B$3:$B$6000,"&lt;"&amp;A$13+1,RawData!$D$3:$D$6000,"="&amp;B$8),MROUND(B$13,1)+1),"")</f>
         <v/>
       </c>
-      <c r="D18" s="28" t="str">
+      <c r="D18" s="27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E18" s="29"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="37" t="str">
+      <c r="E18" s="28"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="36" t="str">
         <f>IF(ISNUMBER(B16),VLOOKUP(B16,RawData!$B$3:$D$6000,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="H18" s="38">
+      <c r="H18" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I18" s="63"/>
+      <c r="I18" s="62"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="39"/>
-      <c r="B19" s="31" t="str">
+      <c r="A19" s="38"/>
+      <c r="B19" s="30" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C19" s="27" t="str">
+      <c r="C19" s="26" t="str">
         <f>IF(ISNUMBER(B19),IF(_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;$B19,RawData!$C$3:$C$6000,"&lt;&gt;"&amp;G21,RawData!$B$3:$B$6000,"&lt;"&amp;A$13+1,RawData!$D$3:$D$6000,"="&amp;B$8)&lt;&gt;0,_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;$B19,RawData!$C$3:$C$6000,"&lt;&gt;"&amp;G21,RawData!$B$3:$B$6000,"&lt;"&amp;A$13+1,RawData!$D$3:$D$6000,"="&amp;B$8),MROUND(B$13,1)+1),"")</f>
         <v/>
       </c>
-      <c r="D19" s="28" t="str">
+      <c r="D19" s="27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E19" s="29"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="37" t="str">
+      <c r="E19" s="28"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="36" t="str">
         <f>IF(ISNUMBER(B17),VLOOKUP(B17,RawData!$B$3:$D$6000,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="H19" s="38">
+      <c r="H19" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="39"/>
-      <c r="B20" s="31" t="str">
+      <c r="A20" s="38"/>
+      <c r="B20" s="30" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C20" s="27" t="str">
+      <c r="C20" s="26" t="str">
         <f>IF(ISNUMBER(B20),IF(_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;$B20,RawData!$C$3:$C$6000,"&lt;&gt;"&amp;G22,RawData!$B$3:$B$6000,"&lt;"&amp;A$13+1,RawData!$D$3:$D$6000,"="&amp;B$8)&lt;&gt;0,_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;$B20,RawData!$C$3:$C$6000,"&lt;&gt;"&amp;G22,RawData!$B$3:$B$6000,"&lt;"&amp;A$13+1,RawData!$D$3:$D$6000,"="&amp;B$8),MROUND(B$13,1)+1),"")</f>
         <v/>
       </c>
-      <c r="D20" s="28" t="str">
+      <c r="D20" s="27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E20" s="29"/>
-      <c r="F20" s="40"/>
-      <c r="G20" s="37" t="str">
+      <c r="E20" s="28"/>
+      <c r="F20" s="39"/>
+      <c r="G20" s="36" t="str">
         <f>IF(ISNUMBER(B18),VLOOKUP(B18,RawData!$B$3:$D$6000,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="H20" s="38">
+      <c r="H20" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I20" s="63"/>
+      <c r="I20" s="62"/>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="39"/>
-      <c r="B21" s="31" t="str">
+      <c r="A21" s="38"/>
+      <c r="B21" s="30" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C21" s="27" t="str">
+      <c r="C21" s="26" t="str">
         <f>IF(ISNUMBER(B21),IF(_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;$B21,RawData!$C$3:$C$6000,"&lt;&gt;"&amp;G23,RawData!$B$3:$B$6000,"&lt;"&amp;A$13+1,RawData!$D$3:$D$6000,"="&amp;B$8)&lt;&gt;0,_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;$B21,RawData!$C$3:$C$6000,"&lt;&gt;"&amp;G23,RawData!$B$3:$B$6000,"&lt;"&amp;A$13+1,RawData!$D$3:$D$6000,"="&amp;B$8),MROUND(B$13,1)+1),"")</f>
         <v/>
       </c>
-      <c r="D21" s="28" t="str">
+      <c r="D21" s="27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E21" s="29"/>
-      <c r="F21" s="40"/>
-      <c r="G21" s="37" t="str">
+      <c r="E21" s="28"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="36" t="str">
         <f>IF(ISNUMBER(B19),VLOOKUP(B19,RawData!$B$3:$D$6000,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="H21" s="38">
+      <c r="H21" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I21" s="63"/>
+      <c r="I21" s="62"/>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="39"/>
-      <c r="B22" s="31" t="str">
+      <c r="A22" s="38"/>
+      <c r="B22" s="30" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C22" s="27" t="str">
+      <c r="C22" s="26" t="str">
         <f>IF(ISNUMBER(B22),IF(_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;$B22,RawData!$C$3:$C$6000,"&lt;&gt;"&amp;G24,RawData!$B$3:$B$6000,"&lt;"&amp;A$13+1,RawData!$D$3:$D$6000,"="&amp;B$8)&lt;&gt;0,_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;$B22,RawData!$C$3:$C$6000,"&lt;&gt;"&amp;G24,RawData!$B$3:$B$6000,"&lt;"&amp;A$13+1,RawData!$D$3:$D$6000,"="&amp;B$8),MROUND(B$13,1)+1),"")</f>
         <v/>
       </c>
-      <c r="D22" s="28" t="str">
+      <c r="D22" s="27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E22" s="29"/>
-      <c r="F22" s="40"/>
-      <c r="G22" s="37" t="str">
+      <c r="E22" s="28"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="36" t="str">
         <f>IF(ISNUMBER(B20),VLOOKUP(B20,RawData!$B$3:$D$6000,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="H22" s="38">
+      <c r="H22" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I22" s="63"/>
+      <c r="I22" s="62"/>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" s="39"/>
-      <c r="B23" s="31" t="str">
+      <c r="A23" s="38"/>
+      <c r="B23" s="30" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C23" s="27" t="str">
+      <c r="C23" s="26" t="str">
         <f>IF(ISNUMBER(B23),IF(_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;$B23,RawData!$C$3:$C$6000,"&lt;&gt;"&amp;G25,RawData!$B$3:$B$6000,"&lt;"&amp;A$13+1,RawData!$D$3:$D$6000,"="&amp;B$8)&lt;&gt;0,_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;$B23,RawData!$C$3:$C$6000,"&lt;&gt;"&amp;G25,RawData!$B$3:$B$6000,"&lt;"&amp;A$13+1,RawData!$D$3:$D$6000,"="&amp;B$8),MROUND(B$13,1)+1),"")</f>
         <v/>
       </c>
-      <c r="D23" s="28" t="str">
+      <c r="D23" s="27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E23" s="29"/>
-      <c r="F23" s="40"/>
-      <c r="G23" s="37" t="str">
+      <c r="E23" s="28"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="36" t="str">
         <f>IF(ISNUMBER(B21),VLOOKUP(B21,RawData!$B$3:$D$6000,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="H23" s="38">
+      <c r="H23" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I23" s="63"/>
+      <c r="I23" s="62"/>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="39"/>
-      <c r="B24" s="31" t="str">
+      <c r="A24" s="38"/>
+      <c r="B24" s="30" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C24" s="27" t="str">
+      <c r="C24" s="26" t="str">
         <f>IF(ISNUMBER(B24),IF(_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;$B24,RawData!$C$3:$C$6000,"&lt;&gt;"&amp;G26,RawData!$B$3:$B$6000,"&lt;"&amp;A$13+1,RawData!$D$3:$D$6000,"="&amp;B$8)&lt;&gt;0,_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;$B24,RawData!$C$3:$C$6000,"&lt;&gt;"&amp;G26,RawData!$B$3:$B$6000,"&lt;"&amp;A$13+1,RawData!$D$3:$D$6000,"="&amp;B$8),MROUND(B$13,1)+1),"")</f>
         <v/>
       </c>
-      <c r="D24" s="28" t="str">
+      <c r="D24" s="27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E24" s="29"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="37" t="str">
+      <c r="E24" s="28"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="36" t="str">
         <f>IF(ISNUMBER(B22),VLOOKUP(B22,RawData!$B$3:$D$6000,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="H24" s="38">
+      <c r="H24" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I24" s="63"/>
+      <c r="I24" s="62"/>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="39"/>
-      <c r="B25" s="31" t="str">
+      <c r="A25" s="38"/>
+      <c r="B25" s="30" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C25" s="27" t="str">
+      <c r="C25" s="26" t="str">
         <f>IF(ISNUMBER(B25),IF(_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;$B25,RawData!$C$3:$C$6000,"&lt;&gt;"&amp;G27,RawData!$B$3:$B$6000,"&lt;"&amp;A$13+1,RawData!$D$3:$D$6000,"="&amp;B$8)&lt;&gt;0,_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;$B25,RawData!$C$3:$C$6000,"&lt;&gt;"&amp;G27,RawData!$B$3:$B$6000,"&lt;"&amp;A$13+1,RawData!$D$3:$D$6000,"="&amp;B$8),MROUND(B$13,1)+1),"")</f>
         <v/>
       </c>
-      <c r="D25" s="28" t="str">
+      <c r="D25" s="27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E25" s="29"/>
-      <c r="F25" s="40"/>
-      <c r="G25" s="37" t="str">
+      <c r="E25" s="28"/>
+      <c r="F25" s="39"/>
+      <c r="G25" s="36" t="str">
         <f>IF(ISNUMBER(B23),VLOOKUP(B23,RawData!$B$3:$D$6000,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="H25" s="38">
+      <c r="H25" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I25" s="63"/>
+      <c r="I25" s="62"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="39"/>
-      <c r="B26" s="31" t="str">
+      <c r="A26" s="38"/>
+      <c r="B26" s="30" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C26" s="27" t="str">
+      <c r="C26" s="26" t="str">
         <f>IF(ISNUMBER(B26),IF(_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;$B26,RawData!$C$3:$C$6000,"&lt;&gt;"&amp;G28,RawData!$B$3:$B$6000,"&lt;"&amp;A$13+1,RawData!$D$3:$D$6000,"="&amp;B$8)&lt;&gt;0,_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;$B26,RawData!$C$3:$C$6000,"&lt;&gt;"&amp;G28,RawData!$B$3:$B$6000,"&lt;"&amp;A$13+1,RawData!$D$3:$D$6000,"="&amp;B$8),MROUND(B$13,1)+1),"")</f>
         <v/>
       </c>
-      <c r="D26" s="28" t="str">
+      <c r="D26" s="27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E26" s="29"/>
-      <c r="F26" s="40"/>
-      <c r="G26" s="37" t="str">
+      <c r="E26" s="28"/>
+      <c r="F26" s="39"/>
+      <c r="G26" s="36" t="str">
         <f>IF(ISNUMBER(B24),VLOOKUP(B24,RawData!$B$3:$D$6000,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="H26" s="38">
+      <c r="H26" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="39"/>
-      <c r="B27" s="31" t="str">
+      <c r="A27" s="38"/>
+      <c r="B27" s="30" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C27" s="27" t="str">
+      <c r="C27" s="26" t="str">
         <f>IF(ISNUMBER(B27),IF(_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;$B27,RawData!$C$3:$C$6000,"&lt;&gt;"&amp;G29,RawData!$B$3:$B$6000,"&lt;"&amp;A$13+1,RawData!$D$3:$D$6000,"="&amp;B$8)&lt;&gt;0,_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;$B27,RawData!$C$3:$C$6000,"&lt;&gt;"&amp;G29,RawData!$B$3:$B$6000,"&lt;"&amp;A$13+1,RawData!$D$3:$D$6000,"="&amp;B$8),MROUND(B$13,1)+1),"")</f>
         <v/>
       </c>
-      <c r="D27" s="28" t="str">
+      <c r="D27" s="27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E27" s="29"/>
-      <c r="F27" s="40"/>
-      <c r="G27" s="37" t="str">
+      <c r="E27" s="28"/>
+      <c r="F27" s="39"/>
+      <c r="G27" s="36" t="str">
         <f>IF(ISNUMBER(B25),VLOOKUP(B25,RawData!$B$3:$D$6000,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="H27" s="38">
+      <c r="H27" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="39"/>
-      <c r="B28" s="31" t="str">
+      <c r="A28" s="38"/>
+      <c r="B28" s="30" t="str">
         <f t="shared" ref="B28:B35" si="3">IF(C27&lt;MROUND(B$13,1)+1,C27,"")</f>
         <v/>
       </c>
-      <c r="C28" s="27" t="str">
+      <c r="C28" s="26" t="str">
         <f>IF(ISNUMBER(B28),IF(_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;$B28,RawData!$C$3:$C$6000,"&lt;&gt;"&amp;G30,RawData!$B$3:$B$6000,"&lt;"&amp;A$13+1,RawData!$D$3:$D$6000,"="&amp;B$8)&lt;&gt;0,_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;$B28,RawData!$C$3:$C$6000,"&lt;&gt;"&amp;G30,RawData!$B$3:$B$6000,"&lt;"&amp;A$13+1,RawData!$D$3:$D$6000,"="&amp;B$8),MROUND(B$13,1)+1),"")</f>
         <v/>
       </c>
-      <c r="D28" s="28" t="str">
+      <c r="D28" s="27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E28" s="29"/>
-      <c r="F28" s="40"/>
-      <c r="G28" s="37" t="str">
+      <c r="E28" s="28"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="36" t="str">
         <f>IF(ISNUMBER(B26),VLOOKUP(B26,RawData!$B$3:$D$6000,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="H28" s="38">
+      <c r="H28" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="41"/>
-      <c r="B29" s="31" t="str">
+      <c r="A29" s="40"/>
+      <c r="B29" s="30" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="C29" s="27" t="str">
+      <c r="C29" s="26" t="str">
         <f>IF(ISNUMBER(B29),IF(_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;$B29,RawData!$C$3:$C$6000,"&lt;&gt;"&amp;G31,RawData!$B$3:$B$6000,"&lt;"&amp;A$13+1,RawData!$D$3:$D$6000,"="&amp;B$8)&lt;&gt;0,_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;$B29,RawData!$C$3:$C$6000,"&lt;&gt;"&amp;G31,RawData!$B$3:$B$6000,"&lt;"&amp;A$13+1,RawData!$D$3:$D$6000,"="&amp;B$8),MROUND(B$13,1)+1),"")</f>
         <v/>
       </c>
-      <c r="D29" s="28" t="str">
+      <c r="D29" s="27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E29" s="29"/>
-      <c r="F29" s="42"/>
-      <c r="G29" s="37" t="str">
+      <c r="E29" s="28"/>
+      <c r="F29" s="41"/>
+      <c r="G29" s="36" t="str">
         <f>IF(ISNUMBER(B27),VLOOKUP(B27,RawData!$B$3:$D$6000,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="H29" s="38">
+      <c r="H29" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="41"/>
-      <c r="B30" s="31" t="str">
+      <c r="A30" s="40"/>
+      <c r="B30" s="30" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="C30" s="27" t="str">
+      <c r="C30" s="26" t="str">
         <f>IF(ISNUMBER(B30),IF(_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;$B30,RawData!$C$3:$C$6000,"&lt;&gt;"&amp;G32,RawData!$B$3:$B$6000,"&lt;"&amp;A$13+1,RawData!$D$3:$D$6000,"="&amp;B$8)&lt;&gt;0,_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;$B30,RawData!$C$3:$C$6000,"&lt;&gt;"&amp;G32,RawData!$B$3:$B$6000,"&lt;"&amp;A$13+1,RawData!$D$3:$D$6000,"="&amp;B$8),MROUND(B$13,1)+1),"")</f>
         <v/>
       </c>
-      <c r="D30" s="28" t="str">
+      <c r="D30" s="27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E30" s="29"/>
-      <c r="F30" s="42"/>
-      <c r="G30" s="37" t="str">
+      <c r="E30" s="28"/>
+      <c r="F30" s="41"/>
+      <c r="G30" s="36" t="str">
         <f>IF(ISNUMBER(B28),VLOOKUP(B28,RawData!$B$3:$D$6000,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="H30" s="38">
+      <c r="H30" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="41"/>
-      <c r="B31" s="31" t="str">
+      <c r="A31" s="40"/>
+      <c r="B31" s="30" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="C31" s="27" t="str">
+      <c r="C31" s="26" t="str">
         <f>IF(ISNUMBER(B31),IF(_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;$B31,RawData!$C$3:$C$6000,"&lt;&gt;"&amp;G33,RawData!$B$3:$B$6000,"&lt;"&amp;A$13+1,RawData!$D$3:$D$6000,"="&amp;B$8)&lt;&gt;0,_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;$B31,RawData!$C$3:$C$6000,"&lt;&gt;"&amp;G33,RawData!$B$3:$B$6000,"&lt;"&amp;A$13+1,RawData!$D$3:$D$6000,"="&amp;B$8),MROUND(B$13,1)+1),"")</f>
         <v/>
       </c>
-      <c r="D31" s="28" t="str">
+      <c r="D31" s="27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E31" s="29"/>
-      <c r="F31" s="42"/>
-      <c r="G31" s="37" t="str">
+      <c r="E31" s="28"/>
+      <c r="F31" s="41"/>
+      <c r="G31" s="36" t="str">
         <f>IF(ISNUMBER(B29),VLOOKUP(B29,RawData!$B$3:$D$6000,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="H31" s="38">
+      <c r="H31" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="41"/>
-      <c r="B32" s="31" t="str">
+      <c r="A32" s="40"/>
+      <c r="B32" s="30" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="C32" s="27" t="str">
+      <c r="C32" s="26" t="str">
         <f>IF(ISNUMBER(B32),IF(_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;$B32,RawData!$C$3:$C$6000,"&lt;&gt;"&amp;G34,RawData!$B$3:$B$6000,"&lt;"&amp;A$13+1,RawData!$D$3:$D$6000,"="&amp;B$8)&lt;&gt;0,_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;$B32,RawData!$C$3:$C$6000,"&lt;&gt;"&amp;G34,RawData!$B$3:$B$6000,"&lt;"&amp;A$13+1,RawData!$D$3:$D$6000,"="&amp;B$8),MROUND(B$13,1)+1),"")</f>
         <v/>
       </c>
-      <c r="D32" s="28" t="str">
+      <c r="D32" s="27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E32" s="29"/>
-      <c r="F32" s="42"/>
-      <c r="G32" s="37" t="str">
+      <c r="E32" s="28"/>
+      <c r="F32" s="41"/>
+      <c r="G32" s="36" t="str">
         <f>IF(ISNUMBER(B30),VLOOKUP(B30,RawData!$B$3:$D$6000,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="H32" s="38">
+      <c r="H32" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="41"/>
-      <c r="B33" s="31" t="str">
+      <c r="A33" s="40"/>
+      <c r="B33" s="30" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="C33" s="27" t="str">
+      <c r="C33" s="26" t="str">
         <f>IF(ISNUMBER(B33),IF(_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;$B33,RawData!$C$3:$C$6000,"&lt;&gt;"&amp;G35,RawData!$B$3:$B$6000,"&lt;"&amp;A$13+1,RawData!$D$3:$D$6000,"="&amp;B$8)&lt;&gt;0,_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;$B33,RawData!$C$3:$C$6000,"&lt;&gt;"&amp;G35,RawData!$B$3:$B$6000,"&lt;"&amp;A$13+1,RawData!$D$3:$D$6000,"="&amp;B$8),MROUND(B$13,1)+1),"")</f>
         <v/>
       </c>
-      <c r="D33" s="28" t="str">
+      <c r="D33" s="27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E33" s="29"/>
-      <c r="F33" s="42"/>
-      <c r="G33" s="37" t="str">
+      <c r="E33" s="28"/>
+      <c r="F33" s="41"/>
+      <c r="G33" s="36" t="str">
         <f>IF(ISNUMBER(B31),VLOOKUP(B31,RawData!$B$3:$D$6000,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="H33" s="38">
+      <c r="H33" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="41"/>
-      <c r="B34" s="31" t="str">
+      <c r="A34" s="40"/>
+      <c r="B34" s="30" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="C34" s="27" t="str">
+      <c r="C34" s="26" t="str">
         <f>IF(ISNUMBER(B34),IF(_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;$B34,RawData!$C$3:$C$6000,"&lt;&gt;"&amp;G36,RawData!$B$3:$B$6000,"&lt;"&amp;A$13+1,RawData!$D$3:$D$6000,"="&amp;B$8)&lt;&gt;0,_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;$B34,RawData!$C$3:$C$6000,"&lt;&gt;"&amp;G36,RawData!$B$3:$B$6000,"&lt;"&amp;A$13+1,RawData!$D$3:$D$6000,"="&amp;B$8),MROUND(B$13,1)+1),"")</f>
         <v/>
       </c>
-      <c r="D34" s="28" t="str">
+      <c r="D34" s="27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E34" s="29"/>
-      <c r="F34" s="42"/>
-      <c r="G34" s="37" t="str">
+      <c r="E34" s="28"/>
+      <c r="F34" s="41"/>
+      <c r="G34" s="36" t="str">
         <f>IF(ISNUMBER(B32),VLOOKUP(B32,RawData!$B$3:$D$6000,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="H34" s="38">
+      <c r="H34" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="39"/>
-      <c r="B35" s="31" t="str">
+      <c r="A35" s="38"/>
+      <c r="B35" s="30" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="C35" s="27" t="str">
+      <c r="C35" s="26" t="str">
         <f>IF(ISNUMBER(B35),IF(_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;$B35,RawData!$C$3:$C$6000,"&lt;&gt;"&amp;G37,RawData!$B$3:$B$6000,"&lt;"&amp;A$13+1,RawData!$D$3:$D$6000,"="&amp;B$8)&lt;&gt;0,_xlfn.MINIFS(RawData!$B$3:$B$6000,RawData!$B$3:$B$6000,"&gt;="&amp;$B35,RawData!$C$3:$C$6000,"&lt;&gt;"&amp;G37,RawData!$B$3:$B$6000,"&lt;"&amp;A$13+1,RawData!$D$3:$D$6000,"="&amp;B$8),MROUND(B$13,1)+1),"")</f>
         <v/>
       </c>
-      <c r="D35" s="28" t="str">
+      <c r="D35" s="27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E35" s="29"/>
-      <c r="F35" s="40"/>
-      <c r="G35" s="37" t="str">
+      <c r="E35" s="28"/>
+      <c r="F35" s="39"/>
+      <c r="G35" s="36" t="str">
         <f>IF(ISNUMBER(B33),VLOOKUP(B33,RawData!$B$3:$D$6000,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="H35" s="38">
+      <c r="H35" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="36" ht="16" customHeight="1" spans="7:11">
-      <c r="G36" s="37" t="str">
+      <c r="G36" s="36" t="str">
         <f>IF(ISNUMBER(B34),VLOOKUP(B34,RawData!$B$3:$D$6000,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="H36" s="38">
+      <c r="H36" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J36" s="55"/>
-      <c r="K36" s="64"/>
+      <c r="J36" s="54"/>
+      <c r="K36" s="63"/>
     </row>
     <row r="37" ht="12" customHeight="1" spans="1:10">
-      <c r="A37" s="43" t="s">
+      <c r="A37" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="B37" s="44"/>
-      <c r="C37" s="45"/>
-      <c r="D37" s="46" t="s">
+      <c r="B37" s="43"/>
+      <c r="C37" s="44"/>
+      <c r="D37" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="E37" s="46"/>
-      <c r="G37" s="37" t="str">
+      <c r="E37" s="45"/>
+      <c r="G37" s="36" t="str">
         <f>IF(ISNUMBER(B35),VLOOKUP(B35,RawData!$B$3:$D$6000,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="H37" s="38">
+      <c r="H37" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J37" s="55"/>
+      <c r="J37" s="54"/>
     </row>
     <row r="38" ht="17" customHeight="1" spans="1:10">
-      <c r="A38" s="47"/>
-      <c r="B38" s="48"/>
-      <c r="C38" s="49"/>
-      <c r="D38" s="50" t="s">
+      <c r="A38" s="46"/>
+      <c r="B38" s="47"/>
+      <c r="C38" s="48"/>
+      <c r="D38" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="E38" s="51"/>
-      <c r="J38" s="55"/>
+      <c r="E38" s="50"/>
+      <c r="J38" s="54"/>
     </row>
     <row r="39" spans="1:10">
-      <c r="A39" s="52" t="s">
+      <c r="A39" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="B39" s="52"/>
-      <c r="C39" s="52"/>
-      <c r="D39" s="53">
+      <c r="B39" s="51"/>
+      <c r="C39" s="51"/>
+      <c r="D39" s="52">
+        <f>SUMIFS(H15:H37,G15:G37,2)</f>
+        <v>0</v>
+      </c>
+      <c r="E39" s="52"/>
+      <c r="F39" s="53"/>
+      <c r="J39" s="54"/>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="B40" s="51"/>
+      <c r="C40" s="51"/>
+      <c r="D40" s="52">
         <f>SUMIFS(H15:H37,G15:G37,1)</f>
         <v>0</v>
       </c>
-      <c r="E39" s="53"/>
-      <c r="F39" s="54"/>
-      <c r="J39" s="55"/>
-    </row>
-    <row r="40" spans="1:10">
-      <c r="A40" s="52" t="s">
-        <v>17</v>
-      </c>
-      <c r="B40" s="52"/>
-      <c r="C40" s="52"/>
-      <c r="D40" s="53">
-        <f>SUMIFS(H15:H37,G15:G37,0)</f>
-        <v>0</v>
-      </c>
-      <c r="E40" s="53"/>
-      <c r="F40" s="54"/>
-      <c r="J40" s="55"/>
+      <c r="E40" s="52"/>
+      <c r="F40" s="53"/>
+      <c r="J40" s="54"/>
     </row>
     <row r="41" spans="10:10">
-      <c r="J41" s="55"/>
+      <c r="J41" s="54"/>
     </row>
     <row r="42" spans="1:10">
-      <c r="A42" s="55"/>
-      <c r="B42" s="55"/>
-      <c r="C42" s="55"/>
-      <c r="D42" s="55"/>
-      <c r="E42" s="55"/>
-      <c r="F42" s="55"/>
-      <c r="G42" s="55"/>
-      <c r="H42" s="55"/>
-      <c r="I42" s="55"/>
-      <c r="J42" s="55"/>
+      <c r="A42" s="54"/>
+      <c r="B42" s="54"/>
+      <c r="C42" s="54"/>
+      <c r="D42" s="54"/>
+      <c r="E42" s="54"/>
+      <c r="F42" s="54"/>
+      <c r="G42" s="54"/>
+      <c r="H42" s="54"/>
+      <c r="I42" s="54"/>
+      <c r="J42" s="54"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="55"/>
-      <c r="B43" s="55"/>
-      <c r="C43" s="55"/>
-      <c r="D43" s="55"/>
-      <c r="E43" s="55"/>
-      <c r="F43" s="55"/>
-      <c r="G43" s="55"/>
-      <c r="H43" s="55"/>
-      <c r="I43" s="55"/>
-      <c r="J43" s="55"/>
+      <c r="A43" s="54"/>
+      <c r="B43" s="54"/>
+      <c r="C43" s="54"/>
+      <c r="D43" s="54"/>
+      <c r="E43" s="54"/>
+      <c r="F43" s="54"/>
+      <c r="G43" s="54"/>
+      <c r="H43" s="54"/>
+      <c r="I43" s="54"/>
+      <c r="J43" s="54"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="55"/>
-      <c r="B44" s="55"/>
-      <c r="C44" s="55"/>
-      <c r="D44" s="55"/>
-      <c r="E44" s="55"/>
-      <c r="F44" s="55"/>
-      <c r="G44" s="55"/>
-      <c r="H44" s="55"/>
-      <c r="I44" s="55"/>
-      <c r="J44" s="55"/>
+      <c r="A44" s="54"/>
+      <c r="B44" s="54"/>
+      <c r="C44" s="54"/>
+      <c r="D44" s="54"/>
+      <c r="E44" s="54"/>
+      <c r="F44" s="54"/>
+      <c r="G44" s="54"/>
+      <c r="H44" s="54"/>
+      <c r="I44" s="54"/>
+      <c r="J44" s="54"/>
     </row>
     <row r="45" spans="1:9">
-      <c r="A45" s="55"/>
-      <c r="B45" s="55"/>
-      <c r="C45" s="55"/>
-      <c r="D45" s="55"/>
-      <c r="E45" s="55"/>
-      <c r="F45" s="55"/>
-      <c r="G45" s="55"/>
-      <c r="H45" s="55"/>
-      <c r="I45" s="55"/>
+      <c r="A45" s="54"/>
+      <c r="B45" s="54"/>
+      <c r="C45" s="54"/>
+      <c r="D45" s="54"/>
+      <c r="E45" s="54"/>
+      <c r="F45" s="54"/>
+      <c r="G45" s="54"/>
+      <c r="H45" s="54"/>
+      <c r="I45" s="54"/>
     </row>
     <row r="46" spans="1:9">
-      <c r="A46" s="55"/>
-      <c r="B46" s="55"/>
-      <c r="C46" s="55"/>
-      <c r="D46" s="55"/>
-      <c r="E46" s="55"/>
-      <c r="F46" s="55"/>
-      <c r="G46" s="55"/>
-      <c r="H46" s="55"/>
-      <c r="I46" s="55"/>
+      <c r="A46" s="54"/>
+      <c r="B46" s="54"/>
+      <c r="C46" s="54"/>
+      <c r="D46" s="54"/>
+      <c r="E46" s="54"/>
+      <c r="F46" s="54"/>
+      <c r="G46" s="54"/>
+      <c r="H46" s="54"/>
+      <c r="I46" s="54"/>
     </row>
     <row r="47" spans="1:9">
-      <c r="A47" s="55"/>
-      <c r="B47" s="55"/>
-      <c r="C47" s="55"/>
-      <c r="D47" s="55"/>
-      <c r="E47" s="55"/>
-      <c r="F47" s="55"/>
-      <c r="G47" s="55"/>
-      <c r="H47" s="55"/>
-      <c r="I47" s="55"/>
+      <c r="A47" s="54"/>
+      <c r="B47" s="54"/>
+      <c r="C47" s="54"/>
+      <c r="D47" s="54"/>
+      <c r="E47" s="54"/>
+      <c r="F47" s="54"/>
+      <c r="G47" s="54"/>
+      <c r="H47" s="54"/>
+      <c r="I47" s="54"/>
     </row>
     <row r="48" spans="1:9">
-      <c r="A48" s="55"/>
-      <c r="B48" s="55"/>
-      <c r="C48" s="55"/>
-      <c r="D48" s="55"/>
-      <c r="E48" s="55"/>
-      <c r="F48" s="55"/>
-      <c r="G48" s="55"/>
-      <c r="H48" s="55"/>
-      <c r="I48" s="55"/>
+      <c r="A48" s="54"/>
+      <c r="B48" s="54"/>
+      <c r="C48" s="54"/>
+      <c r="D48" s="54"/>
+      <c r="E48" s="54"/>
+      <c r="F48" s="54"/>
+      <c r="G48" s="54"/>
+      <c r="H48" s="54"/>
+      <c r="I48" s="54"/>
     </row>
     <row r="49" spans="1:9">
-      <c r="A49" s="55"/>
-      <c r="B49" s="55"/>
-      <c r="C49" s="55"/>
-      <c r="D49" s="55"/>
-      <c r="E49" s="55"/>
-      <c r="F49" s="55"/>
-      <c r="G49" s="55"/>
-      <c r="H49" s="55"/>
-      <c r="I49" s="55"/>
+      <c r="A49" s="54"/>
+      <c r="B49" s="54"/>
+      <c r="C49" s="54"/>
+      <c r="D49" s="54"/>
+      <c r="E49" s="54"/>
+      <c r="F49" s="54"/>
+      <c r="G49" s="54"/>
+      <c r="H49" s="54"/>
+      <c r="I49" s="54"/>
     </row>
     <row r="50" spans="1:9">
-      <c r="A50" s="55"/>
-      <c r="B50" s="55"/>
-      <c r="C50" s="55"/>
-      <c r="D50" s="55"/>
-      <c r="E50" s="55"/>
-      <c r="F50" s="55"/>
-      <c r="G50" s="55"/>
-      <c r="H50" s="55"/>
-      <c r="I50" s="55"/>
+      <c r="A50" s="54"/>
+      <c r="B50" s="54"/>
+      <c r="C50" s="54"/>
+      <c r="D50" s="54"/>
+      <c r="E50" s="54"/>
+      <c r="F50" s="54"/>
+      <c r="G50" s="54"/>
+      <c r="H50" s="54"/>
+      <c r="I50" s="54"/>
     </row>
     <row r="51" spans="1:9">
-      <c r="A51" s="55"/>
-      <c r="B51" s="55"/>
-      <c r="C51" s="55"/>
-      <c r="D51" s="55"/>
-      <c r="E51" s="55"/>
-      <c r="F51" s="55"/>
-      <c r="G51" s="55"/>
-      <c r="H51" s="55"/>
-      <c r="I51" s="55"/>
+      <c r="A51" s="54"/>
+      <c r="B51" s="54"/>
+      <c r="C51" s="54"/>
+      <c r="D51" s="54"/>
+      <c r="E51" s="54"/>
+      <c r="F51" s="54"/>
+      <c r="G51" s="54"/>
+      <c r="H51" s="54"/>
+      <c r="I51" s="54"/>
     </row>
     <row r="52" spans="1:9">
-      <c r="A52" s="55"/>
-      <c r="B52" s="55"/>
-      <c r="C52" s="55"/>
-      <c r="D52" s="55"/>
-      <c r="E52" s="55"/>
-      <c r="F52" s="55"/>
-      <c r="G52" s="55"/>
-      <c r="H52" s="55"/>
-      <c r="I52" s="55"/>
+      <c r="A52" s="54"/>
+      <c r="B52" s="54"/>
+      <c r="C52" s="54"/>
+      <c r="D52" s="54"/>
+      <c r="E52" s="54"/>
+      <c r="F52" s="54"/>
+      <c r="G52" s="54"/>
+      <c r="H52" s="54"/>
+      <c r="I52" s="54"/>
     </row>
     <row r="54" spans="6:6">
-      <c r="F54" s="56"/>
+      <c r="F54" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="36">
@@ -2649,7 +2633,7 @@
   <sheetPr/>
   <dimension ref="B2:H6502"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3:G11"/>
     </sheetView>
   </sheetViews>
@@ -3897,1057 +3881,1057 @@
       <c r="D218" s="2"/>
     </row>
     <row r="219" spans="2:2">
-      <c r="B219" s="4"/>
+      <c r="B219" s="1"/>
     </row>
     <row r="220" spans="2:2">
-      <c r="B220" s="4"/>
+      <c r="B220" s="1"/>
     </row>
     <row r="221" spans="2:2">
-      <c r="B221" s="4"/>
+      <c r="B221" s="1"/>
     </row>
     <row r="222" spans="2:2">
-      <c r="B222" s="4"/>
+      <c r="B222" s="1"/>
     </row>
     <row r="223" spans="2:2">
-      <c r="B223" s="4"/>
+      <c r="B223" s="1"/>
     </row>
     <row r="224" spans="2:2">
-      <c r="B224" s="4"/>
+      <c r="B224" s="1"/>
     </row>
     <row r="225" spans="2:2">
-      <c r="B225" s="4"/>
+      <c r="B225" s="1"/>
     </row>
     <row r="226" spans="2:2">
-      <c r="B226" s="4"/>
+      <c r="B226" s="1"/>
     </row>
     <row r="227" spans="2:2">
-      <c r="B227" s="4"/>
+      <c r="B227" s="1"/>
     </row>
     <row r="228" spans="2:2">
-      <c r="B228" s="4"/>
+      <c r="B228" s="1"/>
     </row>
     <row r="229" spans="2:2">
-      <c r="B229" s="4"/>
+      <c r="B229" s="1"/>
     </row>
     <row r="230" spans="2:2">
-      <c r="B230" s="4"/>
+      <c r="B230" s="1"/>
     </row>
     <row r="231" spans="2:2">
-      <c r="B231" s="4"/>
+      <c r="B231" s="1"/>
     </row>
     <row r="232" spans="2:2">
-      <c r="B232" s="4"/>
+      <c r="B232" s="1"/>
     </row>
     <row r="233" spans="2:2">
-      <c r="B233" s="4"/>
+      <c r="B233" s="1"/>
     </row>
     <row r="234" spans="2:2">
-      <c r="B234" s="4"/>
+      <c r="B234" s="1"/>
     </row>
     <row r="235" spans="2:2">
-      <c r="B235" s="4"/>
+      <c r="B235" s="1"/>
     </row>
     <row r="236" spans="2:2">
-      <c r="B236" s="4"/>
+      <c r="B236" s="1"/>
     </row>
     <row r="237" spans="2:2">
-      <c r="B237" s="4"/>
+      <c r="B237" s="1"/>
     </row>
     <row r="238" spans="2:2">
-      <c r="B238" s="4"/>
+      <c r="B238" s="1"/>
     </row>
     <row r="239" spans="2:2">
-      <c r="B239" s="4"/>
+      <c r="B239" s="1"/>
     </row>
     <row r="240" spans="2:2">
-      <c r="B240" s="4"/>
+      <c r="B240" s="1"/>
     </row>
     <row r="241" spans="2:2">
-      <c r="B241" s="4"/>
+      <c r="B241" s="1"/>
     </row>
     <row r="242" spans="2:2">
-      <c r="B242" s="4"/>
+      <c r="B242" s="1"/>
     </row>
     <row r="243" spans="2:2">
-      <c r="B243" s="4"/>
+      <c r="B243" s="1"/>
     </row>
     <row r="244" spans="2:2">
-      <c r="B244" s="4"/>
+      <c r="B244" s="1"/>
     </row>
     <row r="245" spans="2:2">
-      <c r="B245" s="4"/>
+      <c r="B245" s="1"/>
     </row>
     <row r="246" spans="2:2">
-      <c r="B246" s="4"/>
+      <c r="B246" s="1"/>
     </row>
     <row r="247" spans="2:2">
-      <c r="B247" s="4"/>
+      <c r="B247" s="1"/>
     </row>
     <row r="248" spans="2:2">
-      <c r="B248" s="4"/>
+      <c r="B248" s="1"/>
     </row>
     <row r="249" spans="2:2">
-      <c r="B249" s="4"/>
+      <c r="B249" s="1"/>
     </row>
     <row r="250" spans="2:2">
-      <c r="B250" s="4"/>
+      <c r="B250" s="1"/>
     </row>
     <row r="251" spans="2:2">
-      <c r="B251" s="4"/>
+      <c r="B251" s="1"/>
     </row>
     <row r="252" spans="2:2">
-      <c r="B252" s="4"/>
+      <c r="B252" s="1"/>
     </row>
     <row r="253" spans="2:2">
-      <c r="B253" s="4"/>
+      <c r="B253" s="1"/>
     </row>
     <row r="254" spans="2:2">
-      <c r="B254" s="4"/>
+      <c r="B254" s="1"/>
     </row>
     <row r="255" spans="2:2">
-      <c r="B255" s="4"/>
+      <c r="B255" s="1"/>
     </row>
     <row r="256" spans="2:2">
-      <c r="B256" s="4"/>
+      <c r="B256" s="1"/>
     </row>
     <row r="257" spans="2:2">
-      <c r="B257" s="4"/>
+      <c r="B257" s="1"/>
     </row>
     <row r="258" spans="2:2">
-      <c r="B258" s="4"/>
+      <c r="B258" s="1"/>
     </row>
     <row r="259" spans="2:2">
-      <c r="B259" s="4"/>
+      <c r="B259" s="1"/>
     </row>
     <row r="260" spans="2:2">
-      <c r="B260" s="4"/>
+      <c r="B260" s="1"/>
     </row>
     <row r="261" spans="2:2">
-      <c r="B261" s="4"/>
+      <c r="B261" s="1"/>
     </row>
     <row r="262" spans="2:2">
-      <c r="B262" s="4"/>
+      <c r="B262" s="1"/>
     </row>
     <row r="263" spans="2:2">
-      <c r="B263" s="4"/>
+      <c r="B263" s="1"/>
     </row>
     <row r="264" spans="2:2">
-      <c r="B264" s="4"/>
+      <c r="B264" s="1"/>
     </row>
     <row r="265" spans="2:2">
-      <c r="B265" s="4"/>
+      <c r="B265" s="1"/>
     </row>
     <row r="266" spans="2:2">
-      <c r="B266" s="4"/>
+      <c r="B266" s="1"/>
     </row>
     <row r="267" spans="2:2">
-      <c r="B267" s="4"/>
+      <c r="B267" s="1"/>
     </row>
     <row r="268" spans="2:2">
-      <c r="B268" s="4"/>
+      <c r="B268" s="1"/>
     </row>
     <row r="269" spans="2:2">
-      <c r="B269" s="4"/>
+      <c r="B269" s="1"/>
     </row>
     <row r="270" spans="2:2">
-      <c r="B270" s="4"/>
+      <c r="B270" s="1"/>
     </row>
     <row r="271" spans="2:2">
-      <c r="B271" s="4"/>
+      <c r="B271" s="1"/>
     </row>
     <row r="272" spans="2:2">
-      <c r="B272" s="4"/>
+      <c r="B272" s="1"/>
     </row>
     <row r="273" spans="2:2">
-      <c r="B273" s="4"/>
+      <c r="B273" s="1"/>
     </row>
     <row r="274" spans="2:2">
-      <c r="B274" s="4"/>
+      <c r="B274" s="1"/>
     </row>
     <row r="275" spans="2:2">
-      <c r="B275" s="4"/>
+      <c r="B275" s="1"/>
     </row>
     <row r="276" spans="2:2">
-      <c r="B276" s="4"/>
+      <c r="B276" s="1"/>
     </row>
     <row r="277" spans="2:2">
-      <c r="B277" s="4"/>
+      <c r="B277" s="1"/>
     </row>
     <row r="278" spans="2:2">
-      <c r="B278" s="4"/>
+      <c r="B278" s="1"/>
     </row>
     <row r="279" spans="2:2">
-      <c r="B279" s="4"/>
+      <c r="B279" s="1"/>
     </row>
     <row r="280" spans="2:2">
-      <c r="B280" s="4"/>
+      <c r="B280" s="1"/>
     </row>
     <row r="281" spans="2:2">
-      <c r="B281" s="4"/>
+      <c r="B281" s="1"/>
     </row>
     <row r="282" spans="2:2">
-      <c r="B282" s="4"/>
+      <c r="B282" s="1"/>
     </row>
     <row r="283" spans="2:2">
-      <c r="B283" s="4"/>
+      <c r="B283" s="1"/>
     </row>
     <row r="284" spans="2:2">
-      <c r="B284" s="4"/>
+      <c r="B284" s="1"/>
     </row>
     <row r="285" spans="2:2">
-      <c r="B285" s="4"/>
+      <c r="B285" s="1"/>
     </row>
     <row r="286" spans="2:2">
-      <c r="B286" s="4"/>
+      <c r="B286" s="1"/>
     </row>
     <row r="287" spans="2:2">
-      <c r="B287" s="4"/>
+      <c r="B287" s="1"/>
     </row>
     <row r="288" spans="2:2">
-      <c r="B288" s="4"/>
+      <c r="B288" s="1"/>
     </row>
     <row r="289" spans="2:2">
-      <c r="B289" s="4"/>
+      <c r="B289" s="1"/>
     </row>
     <row r="290" spans="2:2">
-      <c r="B290" s="4"/>
+      <c r="B290" s="1"/>
     </row>
     <row r="291" spans="2:2">
-      <c r="B291" s="4"/>
+      <c r="B291" s="1"/>
     </row>
     <row r="292" spans="2:2">
-      <c r="B292" s="4"/>
+      <c r="B292" s="1"/>
     </row>
     <row r="293" spans="2:2">
-      <c r="B293" s="4"/>
+      <c r="B293" s="1"/>
     </row>
     <row r="294" spans="2:2">
-      <c r="B294" s="4"/>
+      <c r="B294" s="1"/>
     </row>
     <row r="295" spans="2:2">
-      <c r="B295" s="4"/>
+      <c r="B295" s="1"/>
     </row>
     <row r="296" spans="2:2">
-      <c r="B296" s="4"/>
+      <c r="B296" s="1"/>
     </row>
     <row r="297" spans="2:2">
-      <c r="B297" s="4"/>
+      <c r="B297" s="1"/>
     </row>
     <row r="298" spans="2:2">
-      <c r="B298" s="4"/>
+      <c r="B298" s="1"/>
     </row>
     <row r="299" spans="2:2">
-      <c r="B299" s="4"/>
+      <c r="B299" s="1"/>
     </row>
     <row r="300" spans="2:2">
-      <c r="B300" s="4"/>
+      <c r="B300" s="1"/>
     </row>
     <row r="301" spans="2:2">
-      <c r="B301" s="4"/>
+      <c r="B301" s="1"/>
     </row>
     <row r="302" spans="2:2">
-      <c r="B302" s="4"/>
+      <c r="B302" s="1"/>
     </row>
     <row r="303" spans="2:2">
-      <c r="B303" s="4"/>
+      <c r="B303" s="1"/>
     </row>
     <row r="304" spans="2:2">
-      <c r="B304" s="4"/>
+      <c r="B304" s="1"/>
     </row>
     <row r="305" spans="2:2">
-      <c r="B305" s="4"/>
+      <c r="B305" s="1"/>
     </row>
     <row r="306" spans="2:2">
-      <c r="B306" s="4"/>
+      <c r="B306" s="1"/>
     </row>
     <row r="307" spans="2:2">
-      <c r="B307" s="4"/>
+      <c r="B307" s="1"/>
     </row>
     <row r="308" spans="2:2">
-      <c r="B308" s="4"/>
+      <c r="B308" s="1"/>
     </row>
     <row r="309" spans="2:2">
-      <c r="B309" s="4"/>
+      <c r="B309" s="1"/>
     </row>
     <row r="310" spans="2:2">
-      <c r="B310" s="4"/>
+      <c r="B310" s="1"/>
     </row>
     <row r="311" spans="2:2">
-      <c r="B311" s="4"/>
+      <c r="B311" s="1"/>
     </row>
     <row r="312" spans="2:2">
-      <c r="B312" s="4"/>
+      <c r="B312" s="1"/>
     </row>
     <row r="313" spans="2:2">
-      <c r="B313" s="4"/>
+      <c r="B313" s="1"/>
     </row>
     <row r="314" spans="2:2">
-      <c r="B314" s="4"/>
+      <c r="B314" s="1"/>
     </row>
     <row r="315" spans="2:2">
-      <c r="B315" s="4"/>
+      <c r="B315" s="1"/>
     </row>
     <row r="316" spans="2:2">
-      <c r="B316" s="4"/>
+      <c r="B316" s="1"/>
     </row>
     <row r="317" spans="2:2">
-      <c r="B317" s="4"/>
+      <c r="B317" s="1"/>
     </row>
     <row r="318" spans="2:2">
-      <c r="B318" s="4"/>
+      <c r="B318" s="1"/>
     </row>
     <row r="319" spans="2:2">
-      <c r="B319" s="4"/>
+      <c r="B319" s="1"/>
     </row>
     <row r="320" spans="2:2">
-      <c r="B320" s="4"/>
+      <c r="B320" s="1"/>
     </row>
     <row r="321" spans="2:2">
-      <c r="B321" s="4"/>
+      <c r="B321" s="1"/>
     </row>
     <row r="322" spans="2:2">
-      <c r="B322" s="4"/>
+      <c r="B322" s="1"/>
     </row>
     <row r="323" spans="2:2">
-      <c r="B323" s="4"/>
+      <c r="B323" s="1"/>
     </row>
     <row r="324" spans="2:2">
-      <c r="B324" s="4"/>
+      <c r="B324" s="1"/>
     </row>
     <row r="325" spans="2:2">
-      <c r="B325" s="4"/>
+      <c r="B325" s="1"/>
     </row>
     <row r="326" spans="2:2">
-      <c r="B326" s="4"/>
+      <c r="B326" s="1"/>
     </row>
     <row r="327" spans="2:2">
-      <c r="B327" s="4"/>
+      <c r="B327" s="1"/>
     </row>
     <row r="328" spans="2:2">
-      <c r="B328" s="4"/>
+      <c r="B328" s="1"/>
     </row>
     <row r="329" spans="2:2">
-      <c r="B329" s="4"/>
+      <c r="B329" s="1"/>
     </row>
     <row r="330" spans="2:2">
-      <c r="B330" s="4"/>
+      <c r="B330" s="1"/>
     </row>
     <row r="331" spans="2:2">
-      <c r="B331" s="4"/>
+      <c r="B331" s="1"/>
     </row>
     <row r="332" spans="2:2">
-      <c r="B332" s="4"/>
+      <c r="B332" s="1"/>
     </row>
     <row r="333" spans="2:2">
-      <c r="B333" s="4"/>
+      <c r="B333" s="1"/>
     </row>
     <row r="334" spans="2:2">
-      <c r="B334" s="4"/>
+      <c r="B334" s="1"/>
     </row>
     <row r="335" spans="2:2">
-      <c r="B335" s="4"/>
+      <c r="B335" s="1"/>
     </row>
     <row r="336" spans="2:2">
-      <c r="B336" s="4"/>
+      <c r="B336" s="1"/>
     </row>
     <row r="337" spans="2:2">
-      <c r="B337" s="4"/>
+      <c r="B337" s="1"/>
     </row>
     <row r="338" spans="2:2">
-      <c r="B338" s="4"/>
+      <c r="B338" s="1"/>
     </row>
     <row r="339" spans="2:2">
-      <c r="B339" s="4"/>
+      <c r="B339" s="1"/>
     </row>
     <row r="340" spans="2:2">
-      <c r="B340" s="4"/>
+      <c r="B340" s="1"/>
     </row>
     <row r="341" spans="2:2">
-      <c r="B341" s="4"/>
+      <c r="B341" s="1"/>
     </row>
     <row r="342" spans="2:2">
-      <c r="B342" s="4"/>
+      <c r="B342" s="1"/>
     </row>
     <row r="343" spans="2:2">
-      <c r="B343" s="4"/>
+      <c r="B343" s="1"/>
     </row>
     <row r="344" spans="2:2">
-      <c r="B344" s="4"/>
+      <c r="B344" s="1"/>
     </row>
     <row r="345" spans="2:2">
-      <c r="B345" s="4"/>
+      <c r="B345" s="1"/>
     </row>
     <row r="346" spans="2:2">
-      <c r="B346" s="4"/>
+      <c r="B346" s="1"/>
     </row>
     <row r="347" spans="2:2">
-      <c r="B347" s="4"/>
+      <c r="B347" s="1"/>
     </row>
     <row r="348" spans="2:2">
-      <c r="B348" s="4"/>
+      <c r="B348" s="1"/>
     </row>
     <row r="349" spans="2:2">
-      <c r="B349" s="4"/>
+      <c r="B349" s="1"/>
     </row>
     <row r="350" spans="2:2">
-      <c r="B350" s="4"/>
+      <c r="B350" s="1"/>
     </row>
     <row r="351" spans="2:2">
-      <c r="B351" s="4"/>
+      <c r="B351" s="1"/>
     </row>
     <row r="352" spans="2:2">
-      <c r="B352" s="4"/>
+      <c r="B352" s="1"/>
     </row>
     <row r="353" spans="2:2">
-      <c r="B353" s="4"/>
+      <c r="B353" s="1"/>
     </row>
     <row r="354" spans="2:2">
-      <c r="B354" s="4"/>
+      <c r="B354" s="1"/>
     </row>
     <row r="355" spans="2:2">
-      <c r="B355" s="4"/>
+      <c r="B355" s="1"/>
     </row>
     <row r="356" spans="2:2">
-      <c r="B356" s="4"/>
+      <c r="B356" s="1"/>
     </row>
     <row r="357" spans="2:2">
-      <c r="B357" s="4"/>
+      <c r="B357" s="1"/>
     </row>
     <row r="358" spans="2:2">
-      <c r="B358" s="4"/>
+      <c r="B358" s="1"/>
     </row>
     <row r="359" spans="2:2">
-      <c r="B359" s="4"/>
+      <c r="B359" s="1"/>
     </row>
     <row r="360" spans="2:2">
-      <c r="B360" s="4"/>
+      <c r="B360" s="1"/>
     </row>
     <row r="361" spans="2:2">
-      <c r="B361" s="4"/>
+      <c r="B361" s="1"/>
     </row>
     <row r="362" spans="2:2">
-      <c r="B362" s="4"/>
+      <c r="B362" s="1"/>
     </row>
     <row r="363" spans="2:2">
-      <c r="B363" s="4"/>
+      <c r="B363" s="1"/>
     </row>
     <row r="364" spans="2:2">
-      <c r="B364" s="4"/>
+      <c r="B364" s="1"/>
     </row>
     <row r="365" spans="2:2">
-      <c r="B365" s="4"/>
+      <c r="B365" s="1"/>
     </row>
     <row r="366" spans="2:2">
-      <c r="B366" s="4"/>
+      <c r="B366" s="1"/>
     </row>
     <row r="367" spans="2:2">
-      <c r="B367" s="4"/>
+      <c r="B367" s="1"/>
     </row>
     <row r="368" spans="2:2">
-      <c r="B368" s="4"/>
+      <c r="B368" s="1"/>
     </row>
     <row r="369" spans="2:2">
-      <c r="B369" s="4"/>
+      <c r="B369" s="1"/>
     </row>
     <row r="370" spans="2:2">
-      <c r="B370" s="4"/>
+      <c r="B370" s="1"/>
     </row>
     <row r="371" spans="2:2">
-      <c r="B371" s="4"/>
+      <c r="B371" s="1"/>
     </row>
     <row r="372" spans="2:2">
-      <c r="B372" s="4"/>
+      <c r="B372" s="1"/>
     </row>
     <row r="373" spans="2:2">
-      <c r="B373" s="4"/>
+      <c r="B373" s="1"/>
     </row>
     <row r="374" spans="2:2">
-      <c r="B374" s="4"/>
+      <c r="B374" s="1"/>
     </row>
     <row r="375" spans="2:2">
-      <c r="B375" s="4"/>
+      <c r="B375" s="1"/>
     </row>
     <row r="376" spans="2:2">
-      <c r="B376" s="4"/>
+      <c r="B376" s="1"/>
     </row>
     <row r="377" spans="2:2">
-      <c r="B377" s="4"/>
+      <c r="B377" s="1"/>
     </row>
     <row r="378" spans="2:2">
-      <c r="B378" s="4"/>
+      <c r="B378" s="1"/>
     </row>
     <row r="379" spans="2:2">
-      <c r="B379" s="4"/>
+      <c r="B379" s="1"/>
     </row>
     <row r="380" spans="2:2">
-      <c r="B380" s="4"/>
+      <c r="B380" s="1"/>
     </row>
     <row r="381" spans="2:2">
-      <c r="B381" s="4"/>
+      <c r="B381" s="1"/>
     </row>
     <row r="382" spans="2:2">
-      <c r="B382" s="4"/>
+      <c r="B382" s="1"/>
     </row>
     <row r="383" spans="2:2">
-      <c r="B383" s="4"/>
+      <c r="B383" s="1"/>
     </row>
     <row r="384" spans="2:2">
-      <c r="B384" s="4"/>
+      <c r="B384" s="1"/>
     </row>
     <row r="385" spans="2:2">
-      <c r="B385" s="4"/>
+      <c r="B385" s="1"/>
     </row>
     <row r="386" spans="2:2">
-      <c r="B386" s="4"/>
+      <c r="B386" s="1"/>
     </row>
     <row r="387" spans="2:2">
-      <c r="B387" s="4"/>
+      <c r="B387" s="1"/>
     </row>
     <row r="388" spans="2:2">
-      <c r="B388" s="4"/>
+      <c r="B388" s="1"/>
     </row>
     <row r="389" spans="2:2">
-      <c r="B389" s="4"/>
+      <c r="B389" s="1"/>
     </row>
     <row r="390" spans="2:2">
-      <c r="B390" s="4"/>
+      <c r="B390" s="1"/>
     </row>
     <row r="391" spans="2:2">
-      <c r="B391" s="4"/>
+      <c r="B391" s="1"/>
     </row>
     <row r="392" spans="2:2">
-      <c r="B392" s="4"/>
+      <c r="B392" s="1"/>
     </row>
     <row r="393" spans="2:2">
-      <c r="B393" s="4"/>
+      <c r="B393" s="1"/>
     </row>
     <row r="394" spans="2:2">
-      <c r="B394" s="4"/>
+      <c r="B394" s="1"/>
     </row>
     <row r="395" spans="2:2">
-      <c r="B395" s="4"/>
+      <c r="B395" s="1"/>
     </row>
     <row r="396" spans="2:2">
-      <c r="B396" s="4"/>
+      <c r="B396" s="1"/>
     </row>
     <row r="397" spans="2:2">
-      <c r="B397" s="4"/>
+      <c r="B397" s="1"/>
     </row>
     <row r="398" spans="2:2">
-      <c r="B398" s="4"/>
+      <c r="B398" s="1"/>
     </row>
     <row r="399" spans="2:2">
-      <c r="B399" s="4"/>
+      <c r="B399" s="1"/>
     </row>
     <row r="400" spans="2:2">
-      <c r="B400" s="4"/>
+      <c r="B400" s="1"/>
     </row>
     <row r="401" spans="2:2">
-      <c r="B401" s="4"/>
+      <c r="B401" s="1"/>
     </row>
     <row r="402" spans="2:2">
-      <c r="B402" s="4"/>
+      <c r="B402" s="1"/>
     </row>
     <row r="403" spans="2:2">
-      <c r="B403" s="4"/>
+      <c r="B403" s="1"/>
     </row>
     <row r="404" spans="2:2">
-      <c r="B404" s="4"/>
+      <c r="B404" s="1"/>
     </row>
     <row r="405" spans="2:2">
-      <c r="B405" s="4"/>
+      <c r="B405" s="1"/>
     </row>
     <row r="406" spans="2:2">
-      <c r="B406" s="4"/>
+      <c r="B406" s="1"/>
     </row>
     <row r="407" spans="2:2">
-      <c r="B407" s="4"/>
+      <c r="B407" s="1"/>
     </row>
     <row r="408" spans="2:2">
-      <c r="B408" s="4"/>
+      <c r="B408" s="1"/>
     </row>
     <row r="409" spans="2:2">
-      <c r="B409" s="4"/>
+      <c r="B409" s="1"/>
     </row>
     <row r="410" spans="2:2">
-      <c r="B410" s="4"/>
+      <c r="B410" s="1"/>
     </row>
     <row r="411" spans="2:2">
-      <c r="B411" s="4"/>
+      <c r="B411" s="1"/>
     </row>
     <row r="412" spans="2:2">
-      <c r="B412" s="4"/>
+      <c r="B412" s="1"/>
     </row>
     <row r="413" spans="2:2">
-      <c r="B413" s="4"/>
+      <c r="B413" s="1"/>
     </row>
     <row r="414" spans="2:2">
-      <c r="B414" s="4"/>
+      <c r="B414" s="1"/>
     </row>
     <row r="415" spans="2:2">
-      <c r="B415" s="4"/>
+      <c r="B415" s="1"/>
     </row>
     <row r="416" spans="2:2">
-      <c r="B416" s="4"/>
+      <c r="B416" s="1"/>
     </row>
     <row r="417" spans="2:2">
-      <c r="B417" s="4"/>
+      <c r="B417" s="1"/>
     </row>
     <row r="418" spans="2:2">
-      <c r="B418" s="4"/>
+      <c r="B418" s="1"/>
     </row>
     <row r="419" spans="2:2">
-      <c r="B419" s="4"/>
+      <c r="B419" s="1"/>
     </row>
     <row r="420" spans="2:2">
-      <c r="B420" s="4"/>
+      <c r="B420" s="1"/>
     </row>
     <row r="421" spans="2:2">
-      <c r="B421" s="4"/>
+      <c r="B421" s="1"/>
     </row>
     <row r="422" spans="2:2">
-      <c r="B422" s="4"/>
+      <c r="B422" s="1"/>
     </row>
     <row r="423" spans="2:2">
-      <c r="B423" s="4"/>
+      <c r="B423" s="1"/>
     </row>
     <row r="424" spans="2:2">
-      <c r="B424" s="4"/>
+      <c r="B424" s="1"/>
     </row>
     <row r="425" spans="2:2">
-      <c r="B425" s="4"/>
+      <c r="B425" s="1"/>
     </row>
     <row r="426" spans="2:2">
-      <c r="B426" s="4"/>
+      <c r="B426" s="1"/>
     </row>
     <row r="427" spans="2:2">
-      <c r="B427" s="4"/>
+      <c r="B427" s="1"/>
     </row>
     <row r="428" spans="2:2">
-      <c r="B428" s="4"/>
+      <c r="B428" s="1"/>
     </row>
     <row r="429" spans="2:2">
-      <c r="B429" s="4"/>
+      <c r="B429" s="1"/>
     </row>
     <row r="430" spans="2:2">
-      <c r="B430" s="4"/>
+      <c r="B430" s="1"/>
     </row>
     <row r="431" spans="2:2">
-      <c r="B431" s="4"/>
+      <c r="B431" s="1"/>
     </row>
     <row r="432" spans="2:2">
-      <c r="B432" s="4"/>
+      <c r="B432" s="1"/>
     </row>
     <row r="433" spans="2:2">
-      <c r="B433" s="4"/>
+      <c r="B433" s="1"/>
     </row>
     <row r="434" spans="2:2">
-      <c r="B434" s="4"/>
+      <c r="B434" s="1"/>
     </row>
     <row r="435" spans="2:2">
-      <c r="B435" s="4"/>
+      <c r="B435" s="1"/>
     </row>
     <row r="436" spans="2:2">
-      <c r="B436" s="4"/>
+      <c r="B436" s="1"/>
     </row>
     <row r="437" spans="2:2">
-      <c r="B437" s="4"/>
+      <c r="B437" s="1"/>
     </row>
     <row r="438" spans="2:2">
-      <c r="B438" s="4"/>
+      <c r="B438" s="1"/>
     </row>
     <row r="439" spans="2:2">
-      <c r="B439" s="4"/>
+      <c r="B439" s="1"/>
     </row>
     <row r="440" spans="2:2">
-      <c r="B440" s="4"/>
+      <c r="B440" s="1"/>
     </row>
     <row r="441" spans="2:2">
-      <c r="B441" s="4"/>
+      <c r="B441" s="1"/>
     </row>
     <row r="442" spans="2:2">
-      <c r="B442" s="4"/>
+      <c r="B442" s="1"/>
     </row>
     <row r="443" spans="2:2">
-      <c r="B443" s="4"/>
+      <c r="B443" s="1"/>
     </row>
     <row r="444" spans="2:2">
-      <c r="B444" s="4"/>
+      <c r="B444" s="1"/>
     </row>
     <row r="445" spans="2:2">
-      <c r="B445" s="4"/>
+      <c r="B445" s="1"/>
     </row>
     <row r="446" spans="2:2">
-      <c r="B446" s="4"/>
+      <c r="B446" s="1"/>
     </row>
     <row r="447" spans="2:2">
-      <c r="B447" s="4"/>
+      <c r="B447" s="1"/>
     </row>
     <row r="448" spans="2:2">
-      <c r="B448" s="4"/>
+      <c r="B448" s="1"/>
     </row>
     <row r="449" spans="2:2">
-      <c r="B449" s="4"/>
+      <c r="B449" s="1"/>
     </row>
     <row r="450" spans="2:2">
-      <c r="B450" s="4"/>
+      <c r="B450" s="1"/>
     </row>
     <row r="451" spans="2:2">
-      <c r="B451" s="4"/>
+      <c r="B451" s="1"/>
     </row>
     <row r="452" spans="2:2">
-      <c r="B452" s="4"/>
+      <c r="B452" s="1"/>
     </row>
     <row r="453" spans="2:2">
-      <c r="B453" s="4"/>
+      <c r="B453" s="1"/>
     </row>
     <row r="454" spans="2:2">
-      <c r="B454" s="4"/>
+      <c r="B454" s="1"/>
     </row>
     <row r="455" spans="2:2">
-      <c r="B455" s="4"/>
+      <c r="B455" s="1"/>
     </row>
     <row r="456" spans="2:2">
-      <c r="B456" s="4"/>
+      <c r="B456" s="1"/>
     </row>
     <row r="457" spans="2:2">
-      <c r="B457" s="4"/>
+      <c r="B457" s="1"/>
     </row>
     <row r="458" spans="2:2">
-      <c r="B458" s="4"/>
+      <c r="B458" s="1"/>
     </row>
     <row r="459" spans="2:2">
-      <c r="B459" s="4"/>
+      <c r="B459" s="1"/>
     </row>
     <row r="460" spans="2:2">
-      <c r="B460" s="4"/>
+      <c r="B460" s="1"/>
     </row>
     <row r="461" spans="2:2">
-      <c r="B461" s="4"/>
+      <c r="B461" s="1"/>
     </row>
     <row r="462" spans="2:2">
-      <c r="B462" s="4"/>
+      <c r="B462" s="1"/>
     </row>
     <row r="463" spans="2:2">
-      <c r="B463" s="4"/>
+      <c r="B463" s="1"/>
     </row>
     <row r="464" spans="2:2">
-      <c r="B464" s="4"/>
+      <c r="B464" s="1"/>
     </row>
     <row r="465" spans="2:2">
-      <c r="B465" s="4"/>
+      <c r="B465" s="1"/>
     </row>
     <row r="466" spans="2:2">
-      <c r="B466" s="4"/>
+      <c r="B466" s="1"/>
     </row>
     <row r="467" spans="2:2">
-      <c r="B467" s="4"/>
+      <c r="B467" s="1"/>
     </row>
     <row r="468" spans="2:2">
-      <c r="B468" s="4"/>
+      <c r="B468" s="1"/>
     </row>
     <row r="469" spans="2:2">
-      <c r="B469" s="4"/>
+      <c r="B469" s="1"/>
     </row>
     <row r="470" spans="2:2">
-      <c r="B470" s="4"/>
+      <c r="B470" s="1"/>
     </row>
     <row r="471" spans="2:2">
-      <c r="B471" s="4"/>
+      <c r="B471" s="1"/>
     </row>
     <row r="472" spans="2:2">
-      <c r="B472" s="4"/>
+      <c r="B472" s="1"/>
     </row>
     <row r="473" spans="2:2">
-      <c r="B473" s="4"/>
+      <c r="B473" s="1"/>
     </row>
     <row r="474" spans="2:2">
-      <c r="B474" s="4"/>
+      <c r="B474" s="1"/>
     </row>
     <row r="475" spans="2:2">
-      <c r="B475" s="4"/>
+      <c r="B475" s="1"/>
     </row>
     <row r="476" spans="2:2">
-      <c r="B476" s="4"/>
+      <c r="B476" s="1"/>
     </row>
     <row r="477" spans="2:2">
-      <c r="B477" s="4"/>
+      <c r="B477" s="1"/>
     </row>
     <row r="478" spans="2:2">
-      <c r="B478" s="4"/>
+      <c r="B478" s="1"/>
     </row>
     <row r="479" spans="2:2">
-      <c r="B479" s="4"/>
+      <c r="B479" s="1"/>
     </row>
     <row r="480" spans="2:2">
-      <c r="B480" s="4"/>
+      <c r="B480" s="1"/>
     </row>
     <row r="481" spans="2:2">
-      <c r="B481" s="4"/>
+      <c r="B481" s="1"/>
     </row>
     <row r="482" spans="2:2">
-      <c r="B482" s="4"/>
+      <c r="B482" s="1"/>
     </row>
     <row r="483" spans="2:2">
-      <c r="B483" s="4"/>
+      <c r="B483" s="1"/>
     </row>
     <row r="484" spans="2:2">
-      <c r="B484" s="4"/>
+      <c r="B484" s="1"/>
     </row>
     <row r="485" spans="2:2">
-      <c r="B485" s="4"/>
+      <c r="B485" s="1"/>
     </row>
     <row r="486" spans="2:2">
-      <c r="B486" s="4"/>
+      <c r="B486" s="1"/>
     </row>
     <row r="487" spans="2:2">
-      <c r="B487" s="4"/>
+      <c r="B487" s="1"/>
     </row>
     <row r="488" spans="2:2">
-      <c r="B488" s="5"/>
+      <c r="B488" s="4"/>
     </row>
     <row r="489" spans="2:2">
-      <c r="B489" s="5"/>
+      <c r="B489" s="4"/>
     </row>
     <row r="490" spans="2:2">
-      <c r="B490" s="5"/>
+      <c r="B490" s="4"/>
     </row>
     <row r="491" spans="2:2">
-      <c r="B491" s="5"/>
+      <c r="B491" s="4"/>
     </row>
     <row r="492" spans="2:2">
-      <c r="B492" s="5"/>
+      <c r="B492" s="4"/>
     </row>
     <row r="493" spans="2:2">
-      <c r="B493" s="5"/>
+      <c r="B493" s="4"/>
     </row>
     <row r="494" spans="2:2">
-      <c r="B494" s="5"/>
+      <c r="B494" s="4"/>
     </row>
     <row r="495" spans="2:2">
-      <c r="B495" s="5"/>
+      <c r="B495" s="4"/>
     </row>
     <row r="496" spans="2:2">
-      <c r="B496" s="5"/>
+      <c r="B496" s="4"/>
     </row>
     <row r="497" spans="2:2">
-      <c r="B497" s="5"/>
+      <c r="B497" s="4"/>
     </row>
     <row r="498" spans="2:2">
-      <c r="B498" s="5"/>
+      <c r="B498" s="4"/>
     </row>
     <row r="499" spans="2:2">
-      <c r="B499" s="5"/>
+      <c r="B499" s="4"/>
     </row>
     <row r="500" spans="2:2">
-      <c r="B500" s="5"/>
+      <c r="B500" s="4"/>
     </row>
     <row r="501" spans="2:2">
-      <c r="B501" s="5"/>
+      <c r="B501" s="4"/>
     </row>
     <row r="502" spans="2:2">
-      <c r="B502" s="5"/>
+      <c r="B502" s="4"/>
     </row>
     <row r="503" spans="2:2">
-      <c r="B503" s="5"/>
+      <c r="B503" s="4"/>
     </row>
     <row r="504" spans="2:2">
-      <c r="B504" s="5"/>
+      <c r="B504" s="4"/>
     </row>
     <row r="505" spans="2:2">
-      <c r="B505" s="5"/>
+      <c r="B505" s="4"/>
     </row>
     <row r="506" spans="2:2">
-      <c r="B506" s="5"/>
+      <c r="B506" s="4"/>
     </row>
     <row r="507" spans="2:2">
-      <c r="B507" s="5"/>
+      <c r="B507" s="4"/>
     </row>
     <row r="508" spans="2:2">
-      <c r="B508" s="5"/>
+      <c r="B508" s="4"/>
     </row>
     <row r="509" spans="2:2">
-      <c r="B509" s="5"/>
+      <c r="B509" s="4"/>
     </row>
     <row r="510" spans="2:2">
-      <c r="B510" s="5"/>
+      <c r="B510" s="4"/>
     </row>
     <row r="511" spans="2:2">
-      <c r="B511" s="5"/>
+      <c r="B511" s="4"/>
     </row>
     <row r="512" spans="2:2">
-      <c r="B512" s="5"/>
+      <c r="B512" s="4"/>
     </row>
     <row r="513" spans="2:2">
-      <c r="B513" s="5"/>
+      <c r="B513" s="4"/>
     </row>
     <row r="514" spans="2:2">
-      <c r="B514" s="5"/>
+      <c r="B514" s="4"/>
     </row>
     <row r="515" spans="2:2">
-      <c r="B515" s="5"/>
+      <c r="B515" s="4"/>
     </row>
     <row r="516" spans="2:2">
-      <c r="B516" s="5"/>
+      <c r="B516" s="4"/>
     </row>
     <row r="517" spans="2:2">
-      <c r="B517" s="5"/>
+      <c r="B517" s="4"/>
     </row>
     <row r="518" spans="2:2">
-      <c r="B518" s="5"/>
+      <c r="B518" s="4"/>
     </row>
     <row r="519" spans="2:2">
-      <c r="B519" s="5"/>
+      <c r="B519" s="4"/>
     </row>
     <row r="520" spans="2:2">
-      <c r="B520" s="5"/>
+      <c r="B520" s="4"/>
     </row>
     <row r="521" spans="2:2">
-      <c r="B521" s="5"/>
+      <c r="B521" s="4"/>
     </row>
     <row r="522" spans="2:2">
-      <c r="B522" s="5"/>
+      <c r="B522" s="4"/>
     </row>
     <row r="523" spans="2:2">
-      <c r="B523" s="5"/>
+      <c r="B523" s="4"/>
     </row>
     <row r="524" spans="2:2">
-      <c r="B524" s="5"/>
+      <c r="B524" s="4"/>
     </row>
     <row r="525" spans="2:2">
-      <c r="B525" s="5"/>
+      <c r="B525" s="4"/>
     </row>
     <row r="526" spans="2:2">
-      <c r="B526" s="5"/>
+      <c r="B526" s="4"/>
     </row>
     <row r="527" spans="2:2">
-      <c r="B527" s="5"/>
+      <c r="B527" s="4"/>
     </row>
     <row r="528" spans="2:2">
-      <c r="B528" s="5"/>
+      <c r="B528" s="4"/>
     </row>
     <row r="529" spans="2:2">
-      <c r="B529" s="5"/>
+      <c r="B529" s="4"/>
     </row>
     <row r="530" spans="2:2">
-      <c r="B530" s="5"/>
+      <c r="B530" s="4"/>
     </row>
     <row r="531" spans="2:2">
-      <c r="B531" s="5"/>
+      <c r="B531" s="4"/>
     </row>
     <row r="532" spans="2:2">
-      <c r="B532" s="5"/>
+      <c r="B532" s="4"/>
     </row>
     <row r="533" spans="2:2">
-      <c r="B533" s="5"/>
+      <c r="B533" s="4"/>
     </row>
     <row r="534" spans="2:2">
-      <c r="B534" s="5"/>
+      <c r="B534" s="4"/>
     </row>
     <row r="535" spans="2:2">
-      <c r="B535" s="5"/>
+      <c r="B535" s="4"/>
     </row>
     <row r="536" spans="2:2">
-      <c r="B536" s="5"/>
+      <c r="B536" s="4"/>
     </row>
     <row r="537" spans="2:2">
-      <c r="B537" s="5"/>
+      <c r="B537" s="4"/>
     </row>
     <row r="538" spans="2:2">
-      <c r="B538" s="5"/>
+      <c r="B538" s="4"/>
     </row>
     <row r="539" spans="2:2">
-      <c r="B539" s="5"/>
+      <c r="B539" s="4"/>
     </row>
     <row r="540" spans="2:2">
-      <c r="B540" s="5"/>
+      <c r="B540" s="4"/>
     </row>
     <row r="541" spans="2:2">
-      <c r="B541" s="5"/>
+      <c r="B541" s="4"/>
     </row>
     <row r="542" spans="2:2">
-      <c r="B542" s="5"/>
+      <c r="B542" s="4"/>
     </row>
     <row r="543" spans="2:2">
-      <c r="B543" s="5"/>
+      <c r="B543" s="4"/>
     </row>
     <row r="544" spans="2:2">
-      <c r="B544" s="5"/>
+      <c r="B544" s="4"/>
     </row>
     <row r="545" spans="2:2">
-      <c r="B545" s="5"/>
+      <c r="B545" s="4"/>
     </row>
     <row r="546" spans="2:2">
-      <c r="B546" s="5"/>
+      <c r="B546" s="4"/>
     </row>
     <row r="547" spans="2:2">
-      <c r="B547" s="5"/>
+      <c r="B547" s="4"/>
     </row>
     <row r="548" spans="2:2">
-      <c r="B548" s="5"/>
+      <c r="B548" s="4"/>
     </row>
     <row r="549" spans="2:2">
-      <c r="B549" s="5"/>
+      <c r="B549" s="4"/>
     </row>
     <row r="550" spans="2:2">
-      <c r="B550" s="5"/>
+      <c r="B550" s="4"/>
     </row>
     <row r="551" spans="2:2">
-      <c r="B551" s="5"/>
+      <c r="B551" s="4"/>
     </row>
     <row r="552" spans="2:2">
-      <c r="B552" s="5"/>
+      <c r="B552" s="4"/>
     </row>
     <row r="553" spans="2:2">
-      <c r="B553" s="5"/>
+      <c r="B553" s="4"/>
     </row>
     <row r="554" spans="2:2">
-      <c r="B554" s="5"/>
+      <c r="B554" s="4"/>
     </row>
     <row r="555" spans="2:2">
-      <c r="B555" s="5"/>
+      <c r="B555" s="4"/>
     </row>
     <row r="556" spans="2:2">
-      <c r="B556" s="5"/>
+      <c r="B556" s="4"/>
     </row>
     <row r="557" spans="2:2">
-      <c r="B557" s="5"/>
+      <c r="B557" s="4"/>
     </row>
     <row r="558" spans="2:2">
-      <c r="B558" s="5"/>
+      <c r="B558" s="4"/>
     </row>
     <row r="559" spans="2:2">
-      <c r="B559" s="5"/>
+      <c r="B559" s="4"/>
     </row>
     <row r="560" spans="2:2">
-      <c r="B560" s="5"/>
+      <c r="B560" s="4"/>
     </row>
     <row r="561" spans="2:2">
-      <c r="B561" s="5"/>
+      <c r="B561" s="4"/>
     </row>
     <row r="562" spans="2:2">
-      <c r="B562" s="5"/>
+      <c r="B562" s="4"/>
     </row>
     <row r="563" spans="2:2">
-      <c r="B563" s="5"/>
+      <c r="B563" s="4"/>
     </row>
     <row r="564" spans="2:2">
-      <c r="B564" s="5"/>
+      <c r="B564" s="4"/>
     </row>
     <row r="565" spans="2:2">
-      <c r="B565" s="5"/>
+      <c r="B565" s="4"/>
     </row>
     <row r="566" spans="2:2">
-      <c r="B566" s="5"/>
+      <c r="B566" s="4"/>
     </row>
     <row r="567" spans="2:2">
-      <c r="B567" s="5"/>
+      <c r="B567" s="4"/>
     </row>
     <row r="568" spans="2:2">
-      <c r="B568" s="5"/>
+      <c r="B568" s="4"/>
     </row>
     <row r="569" spans="2:2">
-      <c r="B569" s="5"/>
+      <c r="B569" s="4"/>
     </row>
     <row r="570" spans="2:2">
       <c r="B570" s="3"/>

</xml_diff>

<commit_message>
update report template drycon
</commit_message>
<xml_diff>
--- a/Report/drycon.xlsx
+++ b/Report/drycon.xlsx
@@ -1684,7 +1684,7 @@
   <dimension ref="A2:K54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -1773,7 +1773,7 @@
       <c r="H11" s="17"/>
       <c r="I11" s="59"/>
     </row>
-    <row r="12" ht="15.25" spans="1:9">
+    <row r="12" spans="1:9">
       <c r="A12" s="18"/>
       <c r="B12" s="19" t="s">
         <v>11</v>
@@ -1802,7 +1802,7 @@
         <v>1</v>
       </c>
       <c r="D13" s="27" t="str">
-        <f>IF(ISNUMBER(G15),IF(G15=1,"NOT GOOD","GOOD"),"")</f>
+        <f>IF(ISNUMBER(G15),IF(G15=1,"GOOD","NOT GOOD"),"")</f>
         <v/>
       </c>
       <c r="E13" s="28"/>
@@ -1825,7 +1825,7 @@
         <v/>
       </c>
       <c r="D14" s="27" t="str">
-        <f t="shared" ref="D14:D35" si="1">IF(ISNUMBER(G16),IF(G16=1,"NOT GOOD","GOOD"),"")</f>
+        <f>IF(ISNUMBER(G16),IF(G16=1,"GOOD","NOT GOOD"),"")</f>
         <v/>
       </c>
       <c r="E14" s="28"/>
@@ -1845,7 +1845,7 @@
         <v/>
       </c>
       <c r="D15" s="27" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="D15:D35" si="1">IF(ISNUMBER(G17),IF(G17=1,"GOOD","NOT GOOD"),"")</f>
         <v/>
       </c>
       <c r="E15" s="28"/>
@@ -2418,7 +2418,7 @@
       <c r="B39" s="51"/>
       <c r="C39" s="51"/>
       <c r="D39" s="52">
-        <f>SUMIFS(H15:H37,G15:G37,2)</f>
+        <f>SUMIFS(H15:H37,G15:G37,1)</f>
         <v>0</v>
       </c>
       <c r="E39" s="52"/>
@@ -2432,7 +2432,7 @@
       <c r="B40" s="51"/>
       <c r="C40" s="51"/>
       <c r="D40" s="52">
-        <f>SUMIFS(H15:H37,G15:G37,1)</f>
+        <f>SUMIFS(H15:H37,G15:G37,2)</f>
         <v>0</v>
       </c>
       <c r="E40" s="52"/>

</xml_diff>